<commit_message>
add log for this app,use log4net
</commit_message>
<xml_diff>
--- a/doc/功能列表.xlsx
+++ b/doc/功能列表.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>开发功能列表</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -56,6 +56,10 @@
   </si>
   <si>
     <t>序号</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加日志支持</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -216,11 +220,11 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -595,7 +599,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -605,13 +609,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
@@ -698,8 +702,12 @@
       <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>

</xml_diff>